<commit_message>
Adiciona cronograma.xlsx e modifica componetes.xlsx
</commit_message>
<xml_diff>
--- a/componentes.xlsx
+++ b/componentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lesc\Desktop\inversor-documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64AAD6AD-5421-46DE-9E17-1D9F8DBEBEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA5EA14-EB48-481A-BD78-599DB7418927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{55D118FB-C483-4820-B01F-7E53374ED17B}"/>
   </bookViews>
@@ -20,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Item</t>
   </si>
@@ -49,38 +39,78 @@
     <t>Quantidade</t>
   </si>
   <si>
-    <t>Preço</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
     <t>Componentes</t>
   </si>
   <si>
-    <t>Modolu conversor rs485</t>
-  </si>
-  <si>
-    <t>rs485 communication module cfw100</t>
-  </si>
-  <si>
     <t>Carrinho</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>$X</t>
+    <t>Preço (R$)</t>
+  </si>
+  <si>
+    <t>LOJA</t>
+  </si>
+  <si>
+    <t>ViewTech</t>
+  </si>
+  <si>
+    <t>https://www.viewtech.ind.br/modulo-de-expansao-weg-cfw100-crs485-comunicacao</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>https://produto.mercadolivre.com.br/MLB-2655392212-modulo-conversor-bidirecional-rs485-ttl-arduino-pic-rasp-pic-_JM?matt_tool=14213447&amp;matt_word=&amp;matt_source=bing&amp;matt_campaign=MLB_ML_BING_AO_CE-ALL-ALL_X_PLA_ALLB_TXS_ALL&amp;matt_campaign_id=382858295&amp;matt_ad_group=CE&amp;matt_match_type=e&amp;matt_network=o&amp;matt_device=c&amp;matt_keyword=default&amp;msclkid=177180d409fd133f90eee53cb77ef9ed&amp;utm_source=bing&amp;utm_medium=cpc&amp;utm_campaign=MLB_ML_BING_AO_CE-ALL-ALL_X_PLA_ALLB_TXS_ALL&amp;utm_term=4581596253419741&amp;utm_content=CE</t>
+  </si>
+  <si>
+    <t>Transceptor RS485 Arduino</t>
+  </si>
+  <si>
+    <t>RS485 communication module cfw100</t>
+  </si>
+  <si>
+    <t>Mercado Livre</t>
+  </si>
+  <si>
+    <t>Frete (R$)</t>
+  </si>
+  <si>
+    <t>Total (R$)</t>
+  </si>
+  <si>
+    <t>https://produto.mercadolivre.com.br/MLB-2712932646-modulo-wi-fi-esp32-nodemcu-com-bluetooth-38-pinos-_JM?matt_tool=14213447&amp;matt_word=&amp;matt_source=bing&amp;matt_campaign=MLB_ML_BING_AO_CE-ALL-ALL_X_PLA_ALLB_TXS_ALL&amp;matt_campaign_id=382858295&amp;matt_ad_group=CE&amp;matt_match_type=e&amp;matt_network=o&amp;matt_device=c&amp;matt_keyword=default&amp;msclkid=d45d1ae32055141043757f0bf54a32fd&amp;utm_source=bing&amp;utm_medium=cpc&amp;utm_campaign=MLB_ML_BING_AO_CE-ALL-ALL_X_PLA_ALLB_TXS_ALL&amp;utm_term=4581596253419738&amp;utm_content=CE</t>
+  </si>
+  <si>
+    <t>ESP32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,17 +154,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,76 +492,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD5F944-A5ED-4DE7-A974-D16848789B2C}">
-  <dimension ref="D2:I9"/>
+  <dimension ref="D2:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="35.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>7</v>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>15.9</v>
+      </c>
+      <c r="J4" s="4">
+        <v>40</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>8</v>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>419.25</v>
+      </c>
+      <c r="J5" s="4">
+        <v>22</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>47.49</v>
+      </c>
+      <c r="J6" s="4">
+        <v>41</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="F9" s="3">
+        <f>I4+J4+I5+J5+I6+J6</f>
+        <v>585.64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="D2:K2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K5" r:id="rId1" xr:uid="{882275E6-4ECF-4CC2-A0CC-63A2C218FB43}"/>
+    <hyperlink ref="K4" r:id="rId2" display="https://produto.mercadolivre.com.br/MLB-2655392212-modulo-conversor-bidirecional-rs485-ttl-arduino-pic-rasp-pic-_JM?matt_tool=14213447&amp;matt_word=&amp;matt_source=bing&amp;matt_campaign=MLB_ML_BING_AO_CE-ALL-ALL_X_PLA_ALLB_TXS_ALL&amp;matt_campaign_id=382858295&amp;matt_ad_group=CE&amp;matt_match_type=e&amp;matt_network=o&amp;matt_device=c&amp;matt_keyword=default&amp;msclkid=177180d409fd133f90eee53cb77ef9ed&amp;utm_source=bing&amp;utm_medium=cpc&amp;utm_campaign=MLB_ML_BING_AO_CE-ALL-ALL_X_PLA_ALLB_TXS_ALL&amp;utm_term=4581596253419741&amp;utm_content=CE" xr:uid="{910E27EF-06F8-49FF-870A-6D0D119A0EB6}"/>
+    <hyperlink ref="K6" r:id="rId3" display="https://produto.mercadolivre.com.br/MLB-2712932646-modulo-wi-fi-esp32-nodemcu-com-bluetooth-38-pinos-_JM?matt_tool=14213447&amp;matt_word=&amp;matt_source=bing&amp;matt_campaign=MLB_ML_BING_AO_CE-ALL-ALL_X_PLA_ALLB_TXS_ALL&amp;matt_campaign_id=382858295&amp;matt_ad_group=CE&amp;matt_match_type=e&amp;matt_network=o&amp;matt_device=c&amp;matt_keyword=default&amp;msclkid=d45d1ae32055141043757f0bf54a32fd&amp;utm_source=bing&amp;utm_medium=cpc&amp;utm_campaign=MLB_ML_BING_AO_CE-ALL-ALL_X_PLA_ALLB_TXS_ALL&amp;utm_term=4581596253419738&amp;utm_content=CE" xr:uid="{A4978104-7A6A-46FE-9C36-CF3FC1AFA402}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>